<commit_message>
Group work and commenting
</commit_message>
<xml_diff>
--- a/AirportCheckInMeetingNotes.xlsx
+++ b/AirportCheckInMeetingNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Solar\IdeaProjects\PSD2_Group8Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C04D5BF-F732-4158-B4ED-2CB352D12F4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF6AE6F-1D76-4623-B890-0EC8C88F0D23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{C1F31788-D6A8-49D3-99F7-ADB274DE32C1}"/>
+    <workbookView xWindow="16335" yWindow="2925" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="3" xr2:uid="{C1F31788-D6A8-49D3-99F7-ADB274DE32C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Burn Down Chart" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="152">
   <si>
     <t>Week 9 W</t>
   </si>
@@ -326,9 +326,6 @@
     <t>Actual BurnDown</t>
   </si>
   <si>
-    <t>Projected Deadline</t>
-  </si>
-  <si>
     <t xml:space="preserve">Create passenger, test passenger </t>
   </si>
   <si>
@@ -459,6 +456,42 @@
   </si>
   <si>
     <t>Passenter: Account for when the number of passengers becomes too big for an int value</t>
+  </si>
+  <si>
+    <t>TicketBookingSystem: Add error handling for incorrect menu choices (incorrect passenger type, incorrect date)</t>
+  </si>
+  <si>
+    <t>Method Overloading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TicketBookingSystem: Find a better place to save your files </t>
+  </si>
+  <si>
+    <t>Start commenting Adult and Passenger classes</t>
+  </si>
+  <si>
+    <t>Finished Passenger and Adult working code, worked on TicketBookingSystem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Everyone (Melissa Lead) </t>
+  </si>
+  <si>
+    <t>Decided everyone would be better working on it together</t>
+  </si>
+  <si>
+    <t>Finished Child and Senior working code, worked on TicketbookingSystem</t>
+  </si>
+  <si>
+    <t>Start commenting Child and Senior classes and contine write up</t>
+  </si>
+  <si>
+    <t>Finished Plane and Schedule classes, worked on TicketBookingCode. Added comments to all code helped on</t>
+  </si>
+  <si>
+    <t>Work on code documentation and powerpoint presentation</t>
+  </si>
+  <si>
+    <t>Everyone (Ciaran Lead)</t>
   </si>
 </sst>
 </file>
@@ -601,7 +634,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -626,6 +658,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -945,10 +978,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89EAEF8C-9C6D-4416-9398-EC3F7C9DF428}">
-  <dimension ref="B1:P32"/>
+  <dimension ref="B2:P33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,142 +993,118 @@
     <col min="16" max="16" width="73.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B1" s="14" t="s">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="2:16" s="1" customFormat="1" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="16"/>
-      <c r="C2" s="1" t="s">
+    <row r="3" spans="2:16" s="1" customFormat="1" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="B3" s="16"/>
+      <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="15">
+    <row r="4" spans="2:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="15">
         <v>44153</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D4" s="15">
         <v>44155</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E4" s="15">
         <v>44158</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F4" s="15">
         <v>44160</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G4" s="15">
         <v>44162</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H4" s="15">
         <v>44165</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I4" s="15">
         <v>44167</v>
       </c>
-      <c r="J3" s="15">
+      <c r="J4" s="15">
         <v>44169</v>
       </c>
-      <c r="K3" s="15">
+      <c r="K4" s="15">
         <v>44172</v>
       </c>
-      <c r="L3" s="15">
+      <c r="L4" s="15">
         <v>44174</v>
       </c>
-      <c r="M3" s="15">
+      <c r="M4" s="15">
         <v>44176</v>
       </c>
-      <c r="N3" s="15">
+      <c r="N4" s="15">
         <v>44179</v>
       </c>
-      <c r="P3" s="14" t="s">
+      <c r="P4" s="14" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="P4" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="L5" s="19"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
+        <v>5</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
       <c r="P5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -1107,61 +1116,63 @@
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="9"/>
+      <c r="K6" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="L6" s="18"/>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
       <c r="P6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
+      <c r="F7" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="10"/>
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
       <c r="P7" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
+      <c r="F8" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
       <c r="P8" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -1169,21 +1180,21 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
-      <c r="I9" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
+      <c r="I9" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
       <c r="P9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
@@ -1200,55 +1211,56 @@
       <c r="M10" s="9"/>
       <c r="N10" s="9"/>
       <c r="P10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
-        <v>79</v>
+        <v>15</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
-      <c r="F11" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="13" t="s">
+        <v>68</v>
+      </c>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
       <c r="P11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="K12" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
+      <c r="F12" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
       <c r="N12" s="9"/>
       <c r="P12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -1257,20 +1269,19 @@
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="K13" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="L13" s="11"/>
       <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
+      <c r="N13" s="9"/>
       <c r="P13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
@@ -1281,252 +1292,252 @@
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="11" t="s">
+      <c r="L14" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="P14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="P14" t="s">
+      <c r="P15" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="18"/>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="14" t="s">
+    <row r="17" spans="2:16" s="5" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="17"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19" s="14" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="2:16" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="B19" s="16"/>
-      <c r="C19" s="1" t="s">
+    <row r="20" spans="2:16" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="16"/>
+      <c r="C20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="I20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="M20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N19" s="1" t="s">
+      <c r="N20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O19" s="1"/>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C20" s="15">
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C21" s="15">
         <v>44153</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D21" s="15">
         <v>44155</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E21" s="15">
         <v>44158</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F21" s="15">
         <v>44160</v>
       </c>
-      <c r="G20" s="15">
+      <c r="G21" s="15">
         <v>44162</v>
       </c>
-      <c r="H20" s="15">
+      <c r="H21" s="15">
         <v>44165</v>
       </c>
-      <c r="I20" s="15">
+      <c r="I21" s="15">
         <v>44167</v>
       </c>
-      <c r="J20" s="15">
+      <c r="J21" s="15">
         <v>44169</v>
       </c>
-      <c r="K20" s="15">
+      <c r="K21" s="15">
         <v>44172</v>
       </c>
-      <c r="L20" s="15">
+      <c r="L21" s="15">
         <v>44174</v>
       </c>
-      <c r="M20" s="15">
+      <c r="M21" s="15">
         <v>44176</v>
       </c>
-      <c r="N20" s="15">
+      <c r="N21" s="15">
         <v>44179</v>
       </c>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14" t="s">
+      <c r="O21" s="14"/>
+      <c r="P21" s="14" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="P21" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
+        <v>5</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
-      <c r="K22" s="10" t="s">
-        <v>96</v>
-      </c>
+      <c r="K22" s="10"/>
       <c r="L22" s="10"/>
       <c r="M22" s="10"/>
       <c r="N22" s="10"/>
+      <c r="P22" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" s="14" t="s">
-        <v>111</v>
+        <v>10</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="F23" s="10"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="L23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
       <c r="M23" s="10"/>
       <c r="N23" s="10"/>
       <c r="P23" t="s">
-        <v>114</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" s="14" t="s">
-        <v>11</v>
+        <v>110</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
-      <c r="F24" s="12" t="s">
+      <c r="F24" s="10"/>
+      <c r="G24" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="G24" s="12"/>
-      <c r="H24" s="20"/>
+      <c r="H24" s="12"/>
       <c r="I24" s="12"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10" t="s">
-        <v>96</v>
-      </c>
+      <c r="J24" s="12"/>
+      <c r="K24" s="10"/>
       <c r="L24" s="10"/>
       <c r="M24" s="10"/>
       <c r="N24" s="10"/>
+      <c r="P24" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10" t="s">
-        <v>96</v>
-      </c>
+      <c r="F25" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G25" s="12"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="10"/>
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
       <c r="N25" s="10"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
+      <c r="F26" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G26" s="8"/>
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10" t="s">
-        <v>96</v>
-      </c>
+      <c r="J26" s="8"/>
+      <c r="K26" s="10"/>
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10" t="s">
-        <v>96</v>
-      </c>
+      <c r="H27" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="10"/>
       <c r="L27" s="10"/>
       <c r="M27" s="10"/>
       <c r="N27" s="10"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
@@ -1535,77 +1546,72 @@
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10" t="s">
-        <v>96</v>
-      </c>
+      <c r="J28" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="K28" s="13"/>
       <c r="L28" s="10"/>
       <c r="M28" s="10"/>
       <c r="N28" s="10"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B29" s="14" t="s">
-        <v>79</v>
+        <v>15</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
-      <c r="F29" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10" t="s">
-        <v>96</v>
-      </c>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
       <c r="L29" s="10"/>
       <c r="M29" s="10"/>
       <c r="N29" s="10"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B30" s="14" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="L30" s="10"/>
+      <c r="F30" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
       <c r="M30" s="10"/>
       <c r="N30" s="10"/>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="J31" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="K31" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="L31" s="10"/>
+      <c r="F31" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G31" s="11"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
       <c r="M31" s="10"/>
       <c r="N31" s="10"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B32" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
@@ -1613,14 +1619,31 @@
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
+      <c r="K32" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="L32" s="27"/>
+      <c r="M32" s="11"/>
       <c r="N32" s="10"/>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B33" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1631,10 +1654,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54B9472F-3312-437F-805E-9F4AA7CFD1DE}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1653,48 +1676,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="E1" s="26" t="s">
+      <c r="C1" s="26"/>
+      <c r="E1" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="H1" s="26" t="s">
+      <c r="F1" s="26"/>
+      <c r="H1" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="27"/>
-      <c r="K1" s="26" t="s">
+      <c r="I1" s="26"/>
+      <c r="K1" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="27"/>
+      <c r="L1" s="26"/>
     </row>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
       <c r="B2" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>29</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>29</v>
       </c>
       <c r="J2" s="6"/>
       <c r="K2" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>29</v>
@@ -1702,6 +1725,9 @@
       <c r="M2" s="6"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
@@ -1709,13 +1735,16 @@
         <v>32</v>
       </c>
       <c r="I3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="C4" t="s">
         <v>20</v>
       </c>
@@ -1731,7 +1760,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C5" t="s">
         <v>21</v>
@@ -1740,13 +1769,16 @@
         <v>34</v>
       </c>
       <c r="I5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="C6" t="s">
         <v>22</v>
       </c>
@@ -1754,13 +1786,16 @@
         <v>35</v>
       </c>
       <c r="I6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="C7" t="s">
         <v>23</v>
       </c>
@@ -1776,7 +1811,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C8" t="s">
         <v>24</v>
@@ -1785,13 +1820,16 @@
         <v>37</v>
       </c>
       <c r="I8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="C9" t="s">
         <v>25</v>
       </c>
@@ -1806,17 +1844,23 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="C10" t="s">
         <v>26</v>
       </c>
       <c r="F10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="C11" t="s">
         <v>27</v>
       </c>
@@ -1829,7 +1873,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C12" t="s">
         <v>40</v>
@@ -1852,13 +1896,16 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="C15" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C16" t="s">
         <v>47</v>
@@ -1866,7 +1913,7 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C17" t="s">
         <v>48</v>
@@ -1874,7 +1921,7 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C18" t="s">
         <v>49</v>
@@ -1882,23 +1929,34 @@
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C19" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="C20" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1918,7 +1976,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1929,33 +1987,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="23" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="25">
+      <c r="A2" s="24">
         <v>44160</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -1981,103 +2039,121 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="25">
+      <c r="A3" s="24">
         <v>44165</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="7" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="25">
+      <c r="A4" s="24">
         <v>44167</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="24">
+        <v>44169</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="25">
-        <v>44169</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="E5" s="7" t="s">
+    </row>
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="24">
+        <v>44173</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="25">
-        <v>44172</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>134</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="25">
+      <c r="A7" s="24">
         <v>44174</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="25">
+      <c r="A8" s="24">
         <v>44176</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="25">
+      <c r="A9" s="24">
         <v>44179</v>
       </c>
     </row>
@@ -2088,57 +2164,72 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3022955B-6432-47C7-8EE5-B0A3A38B2D96}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>